<commit_message>
implement current limit safety and watchdog, untested
</commit_message>
<xml_diff>
--- a/Calculation Stuff/Stuff.xlsx
+++ b/Calculation Stuff/Stuff.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Dropbox\Dropbox\Work\Flip Clock\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b9977a44478b21da/Documents/GitHub/FlipClock/Calculation Stuff/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D631EC8-766E-4425-B594-7DB6DE09236F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{7D631EC8-766E-4425-B594-7DB6DE09236F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F89BBC63-16A5-4900-B321-DF190B46BED3}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="10245" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{68B55EAD-10D6-4498-B2A9-CE665288B92C}"/>
+    <workbookView xWindow="38280" yWindow="9915" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{68B55EAD-10D6-4498-B2A9-CE665288B92C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Comm type" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1338,7 +1337,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1348,7 +1347,7 @@
         <v>60</v>
       </c>
       <c r="B1">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1371,7 +1370,7 @@
       </c>
       <c r="B3">
         <f>B1/B2</f>
-        <v>4.1666666666666666E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E3" t="s">
         <v>63</v>
@@ -1425,7 +1424,7 @@
       </c>
       <c r="B7">
         <f>B3*B5</f>
-        <v>2.125</v>
+        <v>2.5500000000000003</v>
       </c>
       <c r="E7" t="s">
         <v>66</v>
@@ -1454,7 +1453,7 @@
       </c>
       <c r="B10">
         <f>B3*B6</f>
-        <v>3.0416666666666665</v>
+        <v>3.65</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>